<commit_message>
Updated Test Cases for 7 Segment Adapter and 7 Segment Display
</commit_message>
<xml_diff>
--- a/Documentation/Test_Cases/7_Seg_Adapter_Test_Cases.xlsx
+++ b/Documentation/Test_Cases/7_Seg_Adapter_Test_Cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\God\git\time_travelers_verilog_stopwatch\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010373\git\time_travelers_verilog_stopwatch\Documentation\Test_Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1813D532-B189-4098-A014-DDC2427D94FB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0752831-0935-4558-9B5B-91E27E66EF96}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -325,6 +325,39 @@
 o_digits[7:0] = "11110111" on 4th and 10th millisecond after reset
 o_digits[7:0] = "11101111" on 5th and 11th millisecond after reset
 o_digits[7:0] = "11011111" on 6th and 12th millisecond after reset</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>ae437134060dae78f72575d02b90df204bd349f2</t>
+  </si>
+  <si>
+    <t>ae437134060dae78f72575d02b90df204bd349f3</t>
+  </si>
+  <si>
+    <t>ae437134060dae78f72575d02b90df204bd349f4</t>
+  </si>
+  <si>
+    <t>ae437134060dae78f72575d02b90df204bd349f5</t>
+  </si>
+  <si>
+    <t>ae437134060dae78f72575d02b90df204bd349f6</t>
+  </si>
+  <si>
+    <t>ae437134060dae78f72575d02b90df204bd349f7</t>
+  </si>
+  <si>
+    <t>ae437134060dae78f72575d02b90df204bd349f8</t>
+  </si>
+  <si>
+    <t>ae437134060dae78f72575d02b90df204bd349f9</t>
+  </si>
+  <si>
+    <t>ae437134060dae78f72575d02b90df204bd349f10</t>
+  </si>
+  <si>
+    <t>ae437134060dae78f72575d02b90df204bd349f11</t>
   </si>
 </sst>
 </file>
@@ -374,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -383,6 +416,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,9 +745,9 @@
     <col min="4" max="4" width="36.42578125" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="59" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="45.140625" customWidth="1"/>
     <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -764,8 +798,15 @@
       <c r="F2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -786,6 +827,15 @@
       <c r="F3" t="s">
         <v>35</v>
       </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="227.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -806,6 +856,15 @@
       <c r="F4" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="G4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="213" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -826,6 +885,15 @@
       <c r="F5" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="G5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="216" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -846,6 +914,15 @@
       <c r="F6" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="213" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -866,6 +943,15 @@
       <c r="F7" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="G7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -886,6 +972,15 @@
       <c r="F8" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="G8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -906,6 +1001,15 @@
       <c r="F9" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="G9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -926,6 +1030,15 @@
       <c r="F10" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="G10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -946,18 +1059,46 @@
       <c r="F11" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="G11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H12:I12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="291a90324d5b7e405cdee1cca19d0e54">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a3d94df2e09d7482e07420c2cba8fd2" ns2:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -1103,22 +1244,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA12D9B4-0AFF-4A48-8503-C4B7A72BF3AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{099A5288-121E-4A14-A6B4-83046D76B9FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1134,21 +1277,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA12D9B4-0AFF-4A48-8503-C4B7A72BF3AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>